<commit_message>
edit deletion and addition on project template create trainset
</commit_message>
<xml_diff>
--- a/public/assets/excel-templates/imports/project/project-import.xlsx
+++ b/public/assets/excel-templates/imports/project/project-import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Laravel-proc\rekachain-web\public\assets\excel-templates\imports\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9754AD4E-3A82-4C06-A1CD-783BD07DF991}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C2D61C1-AAC3-4874-A2EA-A5DDE4EB79B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4913BE8E-1EAC-441F-9642-7860F64F0761}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>Nama Proyek</t>
   </si>
@@ -128,26 +128,23 @@
     <t>TS10</t>
   </si>
   <si>
-    <t>kirim data</t>
+    <t>TS11</t>
+  </si>
+  <si>
+    <t>TS12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -241,81 +238,72 @@
 </styleSheet>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>638175</xdr:colOff>
-          <xdr:row>0</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>533400</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2050" name="Button 2" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2050"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002080000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-ID" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Calibri"/>
-                  <a:cs typeface="Calibri"/>
-                </a:rPr>
-                <a:t>Button 2</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData fPrintsWithSheet="0"/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="[0]!SaveAndUpload" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76C3B0AF-6224-4AA7-87E4-F53986928C7D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3505200" y="390525"/>
+          <a:ext cx="1219200" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="id-ID" sz="1100"/>
+            <a:t>KIRIM DATA</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-ID" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -615,12 +603,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157C8442-A386-49FB-AC18-9B151C8FFE57}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157C8442-A386-49FB-AC18-9B151C8FFE57}">
   <sheetPr codeName="ProjectSheet"/>
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,42 +663,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2050" r:id="rId4" name="Button 2">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!SaveAndUpload">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>638175</xdr:colOff>
-                    <xdr:row>0</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>533400</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-  </mc:AlternateContent>
 </worksheet>
 </file>
 
@@ -894,21 +853,21 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5713BF0E-2FF4-40AA-BB0E-1721A8C71424}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="str">
         <f>CONCATENATE("List Trainset Proyek  ", Proyek!B1)</f>
         <v>List Trainset Proyek  612</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
@@ -924,11 +883,8 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
-      <c r="K2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -945,7 +901,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -953,10 +909,10 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -967,7 +923,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -978,7 +934,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -989,7 +945,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1000,7 +956,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1008,10 +964,10 @@
         <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1022,7 +978,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1033,7 +989,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1044,7 +1000,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1052,6 +1008,28 @@
         <v>30</v>
       </c>
       <c r="C13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1071,7 +1049,7 @@
           <x14:formula1>
             <xm:f>'Preset Trainset'!$B$4:$B$9</xm:f>
           </x14:formula1>
-          <xm:sqref>C4 C5 C6 C7 C8 C9 C10 C11 C12 C13</xm:sqref>
+          <xm:sqref>C5 C4 C8 C9 C6 C7 C10 C11 C12 C13 C14 C15</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>